<commit_message>
Filtered Budget and Runtime
Drop TMDB Budget == 0 and Runtime < 60
</commit_message>
<xml_diff>
--- a/3. Data Preparation/Data Description .xlsx
+++ b/3. Data Preparation/Data Description .xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/ee07fcb87baae8af/Documents/GitHub/en553.602.FA23/3. Data Preparation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="56" documentId="8_{9BD653BF-75A1-4DDC-B61F-2D19C19AE170}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{30018BD9-2E2D-4F34-90D3-70CB7E551626}"/>
+  <xr:revisionPtr revIDLastSave="79" documentId="8_{9BD653BF-75A1-4DDC-B61F-2D19C19AE170}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CDECDB63-F053-4639-A151-ABAE14396AD3}"/>
   <bookViews>
-    <workbookView xWindow="2928" yWindow="2928" windowWidth="17280" windowHeight="9444" xr2:uid="{049FCCC7-16CA-44D7-888F-EE7D46C0CE8B}"/>
+    <workbookView xWindow="2562" yWindow="2562" windowWidth="17280" windowHeight="9444" xr2:uid="{049FCCC7-16CA-44D7-888F-EE7D46C0CE8B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="53">
   <si>
     <t>Unnamed: 0</t>
   </si>
@@ -119,9 +119,6 @@
     <t>Release Year</t>
   </si>
   <si>
-    <t>star_scores</t>
-  </si>
-  <si>
     <t>Merged Budget</t>
   </si>
   <si>
@@ -158,9 +155,6 @@
     <t>See Merge Methodology</t>
   </si>
   <si>
-    <t>Engineered</t>
-  </si>
-  <si>
     <t>Variable Name</t>
   </si>
   <si>
@@ -168,6 +162,39 @@
   </si>
   <si>
     <t>hrs mins</t>
+  </si>
+  <si>
+    <t>Raw Star Scores</t>
+  </si>
+  <si>
+    <t>Unweighted Star Score</t>
+  </si>
+  <si>
+    <t>Simple Weight Star Score</t>
+  </si>
+  <si>
+    <t>Log Weight Star Score</t>
+  </si>
+  <si>
+    <t>Exponential Weight Star Score</t>
+  </si>
+  <si>
+    <t>production_company_scores</t>
+  </si>
+  <si>
+    <t>Uniform Sum</t>
+  </si>
+  <si>
+    <t>Linear Weighted Sum</t>
+  </si>
+  <si>
+    <t>Log Weighted Sum</t>
+  </si>
+  <si>
+    <t>Exponential Weighted Sum</t>
+  </si>
+  <si>
+    <t>Array</t>
   </si>
 </sst>
 </file>
@@ -533,10 +560,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6223AA78-8DDC-4145-A31F-67D25DD97AE5}">
-  <dimension ref="A1:C32"/>
+  <dimension ref="A1:C37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="B37" sqref="B1:B37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -547,13 +574,13 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="2" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B1" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>31</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.55000000000000004">
@@ -561,10 +588,10 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.55000000000000004">
@@ -572,10 +599,10 @@
         <v>1</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.55000000000000004">
@@ -583,7 +610,7 @@
         <v>2</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C4" s="1"/>
     </row>
@@ -592,7 +619,7 @@
         <v>3</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C5" s="1"/>
     </row>
@@ -601,10 +628,10 @@
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.55000000000000004">
@@ -612,7 +639,7 @@
         <v>5</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C7" s="1"/>
     </row>
@@ -621,7 +648,7 @@
         <v>6</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C8" s="1"/>
     </row>
@@ -639,7 +666,7 @@
         <v>8</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C10" s="1"/>
     </row>
@@ -648,7 +675,7 @@
         <v>9</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C11" s="1"/>
     </row>
@@ -657,7 +684,7 @@
         <v>10</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C12" s="1"/>
     </row>
@@ -666,7 +693,7 @@
         <v>11</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C13" s="1"/>
     </row>
@@ -675,7 +702,7 @@
         <v>12</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C14" s="1"/>
     </row>
@@ -684,7 +711,7 @@
         <v>13</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C15" s="1"/>
     </row>
@@ -693,7 +720,7 @@
         <v>14</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C16" s="1"/>
     </row>
@@ -711,7 +738,7 @@
         <v>16</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C18" s="1"/>
     </row>
@@ -720,10 +747,10 @@
         <v>17</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.55000000000000004">
@@ -731,7 +758,7 @@
         <v>18</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C20" s="1"/>
     </row>
@@ -740,7 +767,7 @@
         <v>19</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C21" s="1"/>
     </row>
@@ -749,10 +776,10 @@
         <v>20</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.55000000000000004">
@@ -760,10 +787,10 @@
         <v>21</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.55000000000000004">
@@ -771,7 +798,7 @@
         <v>22</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C24" s="1"/>
     </row>
@@ -780,7 +807,7 @@
         <v>23</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C25" s="1"/>
     </row>
@@ -789,7 +816,7 @@
         <v>24</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C26" s="1"/>
     </row>
@@ -798,7 +825,7 @@
         <v>25</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C27" s="1"/>
     </row>
@@ -816,10 +843,10 @@
         <v>27</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.55000000000000004">
@@ -827,32 +854,87 @@
         <v>28</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A31" s="1" t="s">
-        <v>29</v>
+        <v>42</v>
       </c>
       <c r="B31" s="1" t="s">
         <v>34</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>39</v>
+        <v>52</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A32" s="1" t="s">
-        <v>30</v>
+        <v>43</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>40</v>
+        <v>48</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A33" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A34" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A35" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A36" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A37" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>48</v>
       </c>
     </row>
   </sheetData>

</xml_diff>